<commit_message>
implemented simple data transfer
</commit_message>
<xml_diff>
--- a/PropProAssistant/Test/Modelo_BNC.xlsx
+++ b/PropProAssistant/Test/Modelo_BNC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54cd02815d7cac6c/Documentos/Projetos/proppro-assistant/PropProAssistant/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="14_{364F1EDF-D5A2-4785-B6AC-1DA60EAD916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E076919E-F349-42F0-886F-A9B5282E7F8D}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="14_{364F1EDF-D5A2-4785-B6AC-1DA60EAD916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BB2B077-A042-4174-B191-72F899A93678}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,10 +584,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -889,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,6 +2695,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>